<commit_message>
Moved to new dir
</commit_message>
<xml_diff>
--- a/LM-008/Rev C/Project Outputs for LM-008/LM-008.xlsx
+++ b/LM-008/Rev C/Project Outputs for LM-008/LM-008.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43C2EE98-648F-4919-B756-A8F3DF44A085}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70D15E9C-95DE-4C79-AED1-A2F180E79D21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23295" windowHeight="10530" xr2:uid="{10AE6742-50B4-44EB-BA2C-4EC8E2B92281}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23295" windowHeight="10530" xr2:uid="{59940CFD-73D3-4733-97E4-C037C73B34BC}"/>
   </bookViews>
   <sheets>
     <sheet name="LM-008" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="239">
   <si>
     <t>Comment</t>
   </si>
@@ -72,6 +72,9 @@
     <t>Supplier Unit Price 1</t>
   </si>
   <si>
+    <t>SheetNumber</t>
+  </si>
+  <si>
     <t>CAP CER 10UF 6.3V X5R 1206</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
     <t>587-5447-1-ND</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>CAP CER 1UF 50V X7R 1210</t>
   </si>
   <si>
@@ -114,6 +120,9 @@
     <t>490-1863-6-ND</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -138,6 +147,9 @@
     <t>445-14483-6-ND</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -264,6 +276,9 @@
     <t>399-8165-1-ND</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>C16</t>
   </si>
   <si>
@@ -411,31 +426,25 @@
     <t>SAM9597-ND</t>
   </si>
   <si>
-    <t>SSW-115-01-G-D</t>
+    <t xml:space="preserve"> SSW-115-01-F-D</t>
   </si>
   <si>
     <t>Header, 15-Pin, Dual row</t>
   </si>
   <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>HDR2X15</t>
+    <t>P3, P4</t>
+  </si>
+  <si>
+    <t>SSW-115-23-G-D</t>
   </si>
   <si>
     <t>Header 15X2</t>
   </si>
   <si>
-    <t>SAM1208-15-ND</t>
-  </si>
-  <si>
-    <t>SSW-115-21-G-D</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>SSW-115-21-G-D-ND</t>
+    <t>SSW-115-01-F-D</t>
+  </si>
+  <si>
+    <t>SAM10034-ND</t>
   </si>
   <si>
     <t>MCH6336-TL-E</t>
@@ -540,6 +549,9 @@
     <t>CRCW0805100KFKEA/BKN</t>
   </si>
   <si>
+    <t>3, 3, 6</t>
+  </si>
+  <si>
     <t>RES SMD 280K OHM 1% 1/8W 0805</t>
   </si>
   <si>
@@ -576,6 +588,9 @@
     <t/>
   </si>
   <si>
+    <t>5, 5, 6, 6</t>
+  </si>
+  <si>
     <t>LTC4414EMS8#TRPBF</t>
   </si>
   <si>
@@ -660,6 +675,9 @@
     <t>296-36218-1-ND</t>
   </si>
   <si>
+    <t>3, 6</t>
+  </si>
+  <si>
     <t>LT3461</t>
   </si>
   <si>
@@ -702,6 +720,9 @@
     <t>285-2605-ND</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>CCG30-24-12S</t>
   </si>
   <si>
@@ -718,6 +739,9 @@
   </si>
   <si>
     <t>285-2419-ND</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -1111,19 +1135,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B2F992-CACE-4FAE-ACA0-06D51CB6CFFE}">
-  <dimension ref="A1:O38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBE4ACC-CCF7-49BD-9F3F-FA3E3C78FF40}">
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="15" width="14.42578125" customWidth="1"/>
+    <col min="1" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1169,1849 +1192,1910 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M2" s="3">
         <v>4</v>
       </c>
       <c r="N2" s="3">
-        <v>3.09</v>
+        <v>2.7</v>
       </c>
       <c r="O2" s="3">
-        <v>0.20599999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K3" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M3" s="3">
         <v>0</v>
       </c>
       <c r="N3" s="3">
-        <v>4.67</v>
+        <v>3.96</v>
       </c>
       <c r="O3" s="3">
-        <v>0.46700000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.66</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H4" s="3">
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K4" s="3">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="3">
+        <v>3257</v>
+      </c>
+      <c r="N4" s="3">
+        <v>3.42</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="3">
-        <v>35392</v>
-      </c>
-      <c r="N4" s="3">
-        <v>3.8849999999999998</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.25900000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M5" s="3">
-        <v>15312</v>
+        <v>30000</v>
       </c>
       <c r="N5" s="3">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="O5" s="3">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K6" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="M6" s="3">
         <v>40000</v>
       </c>
       <c r="N6" s="3">
-        <v>1.2</v>
+        <v>0.72</v>
       </c>
       <c r="O6" s="3">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K7" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M7" s="3">
-        <v>6077</v>
+        <v>5977</v>
       </c>
       <c r="N7" s="3">
-        <v>0.65</v>
+        <v>0.39</v>
       </c>
       <c r="O7" s="3">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K8" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M8" s="3">
         <v>10000</v>
       </c>
       <c r="N8" s="3">
-        <v>8.3000000000000007</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="O8" s="3">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M9" s="3">
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="O9" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K10" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="M10" s="3">
         <v>0</v>
       </c>
       <c r="N10" s="3">
-        <v>1.05</v>
+        <v>0.63</v>
       </c>
       <c r="O10" s="3">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K11" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="M11" s="3">
         <v>6</v>
       </c>
       <c r="N11" s="3">
-        <v>1.1000000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="O11" s="3">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K12" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="M12" s="3">
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <v>2.0499999999999998</v>
+        <v>1.23</v>
       </c>
       <c r="O12" s="3">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K13" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="M13" s="3">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="N13" s="3">
-        <v>1.85</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="O13" s="3">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H14" s="3">
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K14" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="M14" s="3">
         <v>3000</v>
       </c>
       <c r="N14" s="3">
-        <v>0.75</v>
+        <v>0.45</v>
       </c>
       <c r="O14" s="3">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H15" s="3">
         <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K15" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="M15" s="3">
         <v>0</v>
       </c>
       <c r="N15" s="3">
-        <v>1.45</v>
+        <v>0.87</v>
       </c>
       <c r="O15" s="3">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K16" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="M16" s="3">
         <v>0</v>
       </c>
       <c r="N16" s="3">
-        <v>0.7</v>
+        <v>0.42</v>
       </c>
       <c r="O16" s="3">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K17" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M17" s="3">
-        <v>12018</v>
+        <v>12015</v>
       </c>
       <c r="N17" s="3">
-        <v>2.4500000000000002</v>
+        <v>1.47</v>
       </c>
       <c r="O17" s="3">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K18" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="M18" s="3">
-        <v>637</v>
+        <v>617</v>
       </c>
       <c r="N18" s="3">
-        <v>3.2</v>
+        <v>1.92</v>
       </c>
       <c r="O18" s="3">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H19" s="3">
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K19" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="M19" s="3">
-        <v>14811</v>
+        <v>10811</v>
       </c>
       <c r="N19" s="3">
-        <v>1.65</v>
+        <v>0.99</v>
       </c>
       <c r="O19" s="3">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="H20" s="3">
         <v>2</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K20" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="M20" s="3">
         <v>96</v>
       </c>
       <c r="N20" s="3">
-        <v>25.3</v>
+        <v>15.18</v>
       </c>
       <c r="O20" s="3">
         <v>2.5299999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="G21" s="4" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K21" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="M21" s="3">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="N21" s="3">
-        <v>28.45</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="O21" s="3">
-        <v>5.69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3.07</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K22" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="M22" s="3">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="N22" s="3">
-        <v>23.9</v>
+        <v>4.08</v>
       </c>
       <c r="O22" s="3">
-        <v>4.78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.68</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="H23" s="3">
         <v>2</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K23" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="M23" s="3">
-        <v>3000</v>
+        <v>193467</v>
       </c>
       <c r="N23" s="3">
-        <v>5.69</v>
+        <v>0.6</v>
       </c>
       <c r="O23" s="3">
-        <v>0.56899999999999995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="H24" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K24" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="M24" s="3">
-        <v>203467</v>
+        <v>66</v>
       </c>
       <c r="N24" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.3</v>
       </c>
       <c r="O24" s="3">
-        <v>5.6000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K25" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="M25" s="3">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="N25" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="O25" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="H26" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>21</v>
+        <v>172</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K26" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="M26" s="3">
         <v>0</v>
       </c>
       <c r="N26" s="3">
-        <v>0.5</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="O26" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="3">
         <v>3</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="3">
-        <v>15</v>
-      </c>
       <c r="L27" s="4" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="M27" s="3">
         <v>0</v>
       </c>
-      <c r="N27" s="3">
-        <v>1.53</v>
-      </c>
-      <c r="O27" s="3">
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="H28" s="3">
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K28" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="M28" s="3">
+        <v>32496904</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H29" s="3">
+        <v>4</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="3">
+        <v>6</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="M30" s="3">
         <v>0</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H29" s="3">
+      <c r="N30" s="3">
+        <v>22.74</v>
+      </c>
+      <c r="O30" s="3">
+        <v>3.79</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H31" s="3">
         <v>1</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="3">
-        <v>5</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="M29" s="3">
-        <v>32485423</v>
-      </c>
-      <c r="N29" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O29" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="H30" s="3">
-        <v>4</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H31" s="3">
-        <v>2</v>
-      </c>
       <c r="I31" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K31" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="M31" s="3">
-        <v>314</v>
+        <v>62600</v>
       </c>
       <c r="N31" s="3">
-        <v>37.9</v>
+        <v>1.53</v>
       </c>
       <c r="O31" s="3">
-        <v>3.79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.51</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="H32" s="3">
         <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K32" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="M32" s="3">
-        <v>62807</v>
+        <v>12346</v>
       </c>
       <c r="N32" s="3">
-        <v>2.5499999999999998</v>
+        <v>3.15</v>
       </c>
       <c r="O32" s="3">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.05</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="H33" s="3">
         <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K33" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L33" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="O33" s="3">
+        <v>3.24</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="M33" s="3">
-        <v>12412</v>
-      </c>
-      <c r="N33" s="3">
-        <v>5.25</v>
-      </c>
-      <c r="O33" s="3">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="G34" s="4" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H34" s="3">
+        <v>2</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="3">
+        <v>6</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="M34" s="3">
+        <v>7856</v>
+      </c>
+      <c r="N34" s="3">
+        <v>16.98</v>
+      </c>
+      <c r="O34" s="3">
+        <v>2.83</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H35" s="3">
         <v>1</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K34" s="3">
-        <v>5</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="M34" s="3">
-        <v>0</v>
-      </c>
-      <c r="N34" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="O34" s="3">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="H35" s="3">
-        <v>2</v>
-      </c>
       <c r="I35" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K35" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="M35" s="3">
-        <v>8627</v>
+        <v>56</v>
       </c>
       <c r="N35" s="3">
-        <v>25.41</v>
+        <v>12.06</v>
       </c>
       <c r="O35" s="3">
-        <v>2.5409999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="H36" s="3">
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K36" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="M36" s="3">
-        <v>583</v>
+        <v>31</v>
       </c>
       <c r="N36" s="3">
-        <v>20.100000000000001</v>
+        <v>79.290000000000006</v>
       </c>
       <c r="O36" s="3">
-        <v>4.0199999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26.43</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K37" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="M37" s="3">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="N37" s="3">
-        <v>132.15</v>
+        <v>102</v>
       </c>
       <c r="O37" s="3">
-        <v>26.43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="H38" s="3">
-        <v>1</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K38" s="3">
-        <v>5</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="M38" s="3">
-        <v>287</v>
-      </c>
-      <c r="N38" s="3">
-        <v>170</v>
-      </c>
-      <c r="O38" s="3">
         <v>34</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="Component" display="'Taiyo Yuden" xr:uid="{A75D46E4-E2CE-4C78-B049-C326EA5EE244}"/>
-    <hyperlink ref="G2" r:id="rId2" tooltip="Manufacturer" display="'JMK316BJ106ML-T" xr:uid="{A03E84D3-9257-4DDF-80EA-7A054352DB52}"/>
-    <hyperlink ref="L2" r:id="rId3" tooltip="Supplier" display="'587-5447-1-ND" xr:uid="{663F5BCF-1E6A-4EDB-8A1A-F29514719ECB}"/>
-    <hyperlink ref="F3" r:id="rId4" tooltip="Component" display="'Murata Electronics North America" xr:uid="{DACACD24-5693-42BF-98B7-7FF8820189BF}"/>
-    <hyperlink ref="G3" r:id="rId5" tooltip="Manufacturer" display="'GRM32RR71H105KA01L" xr:uid="{FA8C3567-50C1-44FC-A134-444FFDC630DC}"/>
-    <hyperlink ref="L3" r:id="rId6" tooltip="Supplier" display="'490-1863-6-ND" xr:uid="{110BC81A-DC78-4C03-BF1D-C92C3D1A26E5}"/>
-    <hyperlink ref="F4" r:id="rId7" tooltip="Component" display="'TDK Corporation" xr:uid="{FE575021-3849-4965-AF2F-D1BE80684A7E}"/>
-    <hyperlink ref="G4" r:id="rId8" tooltip="Manufacturer" display="'C2012X6S1C106K085AC" xr:uid="{D0C7BD96-CA31-4D48-92CD-CC0FB4997162}"/>
-    <hyperlink ref="L4" r:id="rId9" tooltip="Supplier" display="'445-14483-6-ND" xr:uid="{5B596A2A-D026-4F0E-845B-7597E8BA879E}"/>
-    <hyperlink ref="F5" r:id="rId10" tooltip="Component" display="'Yageo" xr:uid="{52047C9C-EBAB-4A22-B194-B4478D5FA58E}"/>
-    <hyperlink ref="G5" r:id="rId11" tooltip="Manufacturer" display="'CC0805KKX7R6BB105" xr:uid="{7407D902-73ED-4010-A0CC-D9FD26C0E775}"/>
-    <hyperlink ref="L5" r:id="rId12" tooltip="Supplier" display="'311-1458-6-ND" xr:uid="{77884873-2CB7-48C6-B34E-AE9D9143B292}"/>
-    <hyperlink ref="F6" r:id="rId13" tooltip="Component" display="'TDK Corporation" xr:uid="{1ACCC905-D50F-4D02-BB12-E6F30983BFAE}"/>
-    <hyperlink ref="G6" r:id="rId14" tooltip="Manufacturer" display="'C1608X5R1H684K080AB" xr:uid="{DA2FE4E3-0145-4882-9A83-6BF9351C731F}"/>
-    <hyperlink ref="L6" r:id="rId15" tooltip="Supplier" display="'445-7466-6-ND" xr:uid="{7B83FC98-0AE6-4D73-BC0C-6818FFCCD4EC}"/>
-    <hyperlink ref="F7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{1C5D9529-2AF2-4E86-86AF-1DE02744D19D}"/>
-    <hyperlink ref="G7" r:id="rId17" tooltip="Manufacturer" display="'C0805C100M4GACTU" xr:uid="{1FB59B3F-223B-4865-A21B-FB2B8D5285AC}"/>
-    <hyperlink ref="L7" r:id="rId18" tooltip="Supplier" display="'399-9147-6-ND" xr:uid="{544EBD15-EE0A-40DD-AF76-31B79FFE6CEB}"/>
-    <hyperlink ref="F8" r:id="rId19" tooltip="Component" display="'Murata Electronics North America" xr:uid="{E60F6310-7181-4E31-B38D-B86D970FE009}"/>
-    <hyperlink ref="G8" r:id="rId20" tooltip="Manufacturer" display="'GRM32ER71H475KA88L" xr:uid="{CE0DED92-186A-462F-9FD5-FCFDFEDDE7BB}"/>
-    <hyperlink ref="L8" r:id="rId21" tooltip="Supplier" display="'490-1864-6-ND" xr:uid="{452132C7-C090-4EA1-BBCD-609E61C4ACB1}"/>
-    <hyperlink ref="F9" r:id="rId22" tooltip="Component" display="'TDK Corporation" xr:uid="{85DE70AF-D31A-4A60-86BB-1A0411913854}"/>
-    <hyperlink ref="G9" r:id="rId23" tooltip="Manufacturer" display="'C1608X5R1H104K080AA" xr:uid="{12F5C5CB-8600-4FFC-BE47-273479FD350D}"/>
-    <hyperlink ref="L9" r:id="rId24" tooltip="Supplier" display="'445-7456-6-ND" xr:uid="{5BCB76DD-0E86-4B3E-B83E-CC922FDE8E60}"/>
-    <hyperlink ref="F10" r:id="rId25" tooltip="Component" display="'Murata Electronics North America" xr:uid="{519E362E-AC25-4CD5-84C9-46DD6C55EFB4}"/>
-    <hyperlink ref="G10" r:id="rId26" tooltip="Manufacturer" display="'GRM188R61A225KE34D" xr:uid="{76009C99-D0C3-4D95-86F2-13A6D7CEC71E}"/>
-    <hyperlink ref="L10" r:id="rId27" tooltip="Supplier" display="'490-1545-6-ND" xr:uid="{112CD1CF-7C10-41F9-87EB-1842C980326B}"/>
-    <hyperlink ref="F11" r:id="rId28" tooltip="Component" display="'KEMET" xr:uid="{0F17EF06-DA7A-43C3-8AAA-1264179A9097}"/>
-    <hyperlink ref="G11" r:id="rId29" tooltip="Manufacturer" display="'C1206C220K5GACTU" xr:uid="{79926406-A908-4AF5-A0FD-C78895FEDEB2}"/>
-    <hyperlink ref="L11" r:id="rId30" tooltip="Supplier" display="'399-8165-1-ND" xr:uid="{2B194E3F-4A32-4FFB-BFC4-1FDB7F8425E3}"/>
-    <hyperlink ref="F12" r:id="rId31" tooltip="Component" display="'Taiyo Yuden" xr:uid="{7093A2B8-C667-436D-8CCD-551F39E40901}"/>
-    <hyperlink ref="G12" r:id="rId32" tooltip="Manufacturer" display="'UMK325B7105KH-T" xr:uid="{A81CD794-A29B-466E-9F2C-2C7EE304C4A2}"/>
-    <hyperlink ref="L12" r:id="rId33" tooltip="Supplier" display="'587-1366-1-ND" xr:uid="{1FD4FD6E-AF75-4813-99A1-5488FE997062}"/>
-    <hyperlink ref="F13" r:id="rId34" tooltip="Component" display="'Taiyo Yuden" xr:uid="{C796E4ED-5CFC-4D20-B1A2-77D92CFD54BB}"/>
-    <hyperlink ref="G13" r:id="rId35" tooltip="Manufacturer" display="'UMK316B7474KL-T" xr:uid="{5626EFE8-BA3D-4049-AEBE-AD8D1F8CF655}"/>
-    <hyperlink ref="L13" r:id="rId36" tooltip="Supplier" display="'587-1325-1-ND" xr:uid="{357E22FF-1AE8-4C22-8C79-8D658C54EF7A}"/>
-    <hyperlink ref="F14" r:id="rId37" tooltip="Component" display="'Taiyo Yuden" xr:uid="{FBB19D87-8AA9-4CAA-AD54-30D347011788}"/>
-    <hyperlink ref="G14" r:id="rId38" tooltip="Manufacturer" display="'EMK212B7105KG-T" xr:uid="{523123B3-DA84-46FB-ADE0-96C2C5F9C003}"/>
-    <hyperlink ref="L14" r:id="rId39" tooltip="Supplier" display="'587-1283-1-ND" xr:uid="{C2B27ADA-CA25-4907-8C22-B348A2116199}"/>
-    <hyperlink ref="F15" r:id="rId40" tooltip="Component" display="'KEMET" xr:uid="{8A1583A2-0AC7-4DFF-AF94-1126FC3FAB04}"/>
-    <hyperlink ref="G15" r:id="rId41" tooltip="Manufacturer" display="'C0805C475K4RACTU" xr:uid="{AA4D6721-7966-4014-A494-DBF958BDCDC9}"/>
-    <hyperlink ref="L15" r:id="rId42" tooltip="Supplier" display="'399-7415-1-ND" xr:uid="{5EC5DD64-2C77-43D2-944E-705BA804C971}"/>
-    <hyperlink ref="F16" r:id="rId43" tooltip="Component" display="'Murata Electronics North America" xr:uid="{BF750FEB-558F-44E0-B657-719D0B54C12D}"/>
-    <hyperlink ref="G16" r:id="rId44" tooltip="Manufacturer" display="'GRM188R71C473KA01D" xr:uid="{579BDC68-2CD0-48BF-ABCF-24EDBDCFEFA8}"/>
-    <hyperlink ref="L16" r:id="rId45" tooltip="Supplier" display="'490-1529-6-ND" xr:uid="{B05090A1-7FCE-47DB-B50C-A41C961FF7A1}"/>
-    <hyperlink ref="F17" r:id="rId46" tooltip="Component" display="'Comchip Technology" xr:uid="{2C6C52E1-A6D0-47AC-A320-43103F975F56}"/>
-    <hyperlink ref="G17" r:id="rId47" tooltip="Manufacturer" display="'CDBA540-HF" xr:uid="{7985E781-6943-42AD-9EF0-99A8E9D0395B}"/>
-    <hyperlink ref="L17" r:id="rId48" tooltip="Supplier" display="'641-1707-6-ND" xr:uid="{B004A1E1-E6A8-4F76-9108-5798CFD25249}"/>
-    <hyperlink ref="F18" r:id="rId49" tooltip="Component" display="'Pulse Electronics Power" xr:uid="{1CCE4DE9-BF6A-4FFC-BBDD-EB13104C7AC9}"/>
-    <hyperlink ref="G18" r:id="rId50" tooltip="Manufacturer" display="'PA4332.222NLT" xr:uid="{547C959E-09C7-4C7B-AF83-CDC6DC63AC25}"/>
-    <hyperlink ref="L18" r:id="rId51" tooltip="Supplier" display="'553-3290-6-ND" xr:uid="{1BA408AC-0E89-450B-99D6-BA2102830FD5}"/>
-    <hyperlink ref="F19" r:id="rId52" tooltip="Component" display="'Murata Electronics North America" xr:uid="{C583AE35-DBD2-421A-8363-06469C1FCB48}"/>
-    <hyperlink ref="G19" r:id="rId53" tooltip="Manufacturer" display="'LQH32CN470K23L" xr:uid="{A0D0774E-410E-430D-BD0D-106A99BDECB8}"/>
-    <hyperlink ref="L19" r:id="rId54" tooltip="Supplier" display="'490-2497-1-ND" xr:uid="{2A07A43A-02B2-4D56-8138-904FCC63E677}"/>
-    <hyperlink ref="F20" r:id="rId55" tooltip="Component" display="'Samtec Inc." xr:uid="{5E0D32D2-166A-4B48-A610-157591BD7F1B}"/>
-    <hyperlink ref="G20" r:id="rId56" tooltip="Manufacturer" display="'IPL1-104-01-L-S-RA-K" xr:uid="{93456F34-9EE5-4F3E-9D38-3E3675CF4E26}"/>
-    <hyperlink ref="L20" r:id="rId57" tooltip="Supplier" display="'SAM9597-ND" xr:uid="{BB7F0AA0-9F2C-4016-A871-A9018B35AAC6}"/>
-    <hyperlink ref="F21" r:id="rId58" tooltip="Component" display="'Samtec Inc." xr:uid="{BEC4F0E5-373B-4E81-B202-E6C27B327C6C}"/>
-    <hyperlink ref="G21" r:id="rId59" tooltip="Manufacturer" display="'SSW-115-01-G-D" xr:uid="{EAC94DD6-344C-4ADA-A40D-49C1C307855B}"/>
-    <hyperlink ref="L21" r:id="rId60" tooltip="Supplier" display="'SAM1208-15-ND" xr:uid="{57B4181A-CBF1-4542-8C9A-B0D7D58E8532}"/>
-    <hyperlink ref="F22" r:id="rId61" tooltip="Component" display="'Samtec Inc." xr:uid="{72D6A6A9-F0B6-4780-BE7C-65F9960F38EF}"/>
-    <hyperlink ref="G22" r:id="rId62" tooltip="Manufacturer" display="'SSW-115-21-G-D" xr:uid="{7ECFB409-7D28-4F79-AC13-0C2B7A07BC40}"/>
-    <hyperlink ref="L22" r:id="rId63" tooltip="Supplier" display="'SSW-115-21-G-D-ND" xr:uid="{2BFC99E6-8DC6-424E-A139-FDBAAC509A5C}"/>
-    <hyperlink ref="F23" r:id="rId64" tooltip="Component" display="'ON Semiconductor" xr:uid="{8D2EE353-69C6-4A66-AB2B-8B8635BD57F0}"/>
-    <hyperlink ref="G23" r:id="rId65" tooltip="Manufacturer" display="'MCH6336-TL-E" xr:uid="{093A397A-0B68-4FA4-9CAD-A84ECD127A71}"/>
-    <hyperlink ref="L23" r:id="rId66" tooltip="Supplier" display="'MCH6336-TL-EOSCT-ND" xr:uid="{73B005EB-5767-49F2-9D53-9C8BA9365A84}"/>
-    <hyperlink ref="F24" r:id="rId67" tooltip="Component" display="'Panasonic Electronic Components" xr:uid="{8FBFD0B0-0A98-4BDC-A8BB-FC12816901D0}"/>
-    <hyperlink ref="G24" r:id="rId68" tooltip="Manufacturer" display="'ERJ-2RKF5603X" xr:uid="{96D8BAC7-81A7-4F6F-80E1-88CE33DCF392}"/>
-    <hyperlink ref="L24" r:id="rId69" tooltip="Supplier" display="'P560KLCT-ND" xr:uid="{6F680FD7-0D06-45F6-A9BA-CFFABA0B7D06}"/>
-    <hyperlink ref="F25" r:id="rId70" tooltip="Component" display="'Vishay Dale" xr:uid="{C0C2AF65-9154-44B2-9F7B-A4BA65CDDF24}"/>
-    <hyperlink ref="G25" r:id="rId71" tooltip="Manufacturer" display="'CRCW080588K7FKEA" xr:uid="{A45B0EA5-FDDB-4BA9-87E0-2A05C76BAE84}"/>
-    <hyperlink ref="L25" r:id="rId72" tooltip="Supplier" display="'541-88.7KCDKR-ND" xr:uid="{FF3BF68E-B0E0-4B9F-A3F6-FCAB2722E4B8}"/>
-    <hyperlink ref="F26" r:id="rId73" tooltip="Component" display="'Vishay Dale" xr:uid="{9EA8EDC2-B170-4EDB-876A-0AD044C771D8}"/>
-    <hyperlink ref="G26" r:id="rId74" tooltip="Manufacturer" display="'CRCW080522K1FKEA" xr:uid="{EBE80D94-B665-46AF-BBD0-B6DB5D46A53F}"/>
-    <hyperlink ref="L26" r:id="rId75" tooltip="Supplier" display="'541-22.1KCDKR-ND" xr:uid="{D90C1E1C-72ED-4719-BC7E-576D472A60A1}"/>
-    <hyperlink ref="F27" r:id="rId76" tooltip="Component" display="'Vishay" xr:uid="{9CBB0117-2980-4ED0-9CFD-96A88C79AA96}"/>
-    <hyperlink ref="G27" r:id="rId77" tooltip="Manufacturer" display="'CRCW0805100KFKEA" xr:uid="{ED3CFD53-F416-4AFC-A21D-240139E494DC}"/>
-    <hyperlink ref="L27" r:id="rId78" tooltip="Supplier" display="'CRCW0805100KFKEA/BKN" xr:uid="{BFFC869A-9443-41C8-901C-DAA314EDC4D9}"/>
-    <hyperlink ref="F28" r:id="rId79" tooltip="Component" display="'Vishay Dale" xr:uid="{CCC7A881-A1F1-47C8-B720-EED463D52DC8}"/>
-    <hyperlink ref="G28" r:id="rId80" tooltip="Manufacturer" display="'CRCW0805280KFKEA" xr:uid="{AB9BF7C1-FFD0-418E-858F-DDB10EE366C1}"/>
-    <hyperlink ref="L28" r:id="rId81" tooltip="Supplier" display="'541-280KCTR-ND" xr:uid="{148B3CBF-C5FE-4AC0-B68D-3FAEE4E8D0D5}"/>
-    <hyperlink ref="F29" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{672A7B97-293C-4BC3-AA9D-B3DBA2D3D891}"/>
-    <hyperlink ref="G29" r:id="rId83" tooltip="Manufacturer" display="'RC0805FR-0710KL" xr:uid="{9A5D0D9B-E103-4829-862F-C3BFFC32421E}"/>
-    <hyperlink ref="L29" r:id="rId84" tooltip="Supplier" display="'311-10.0KCRCT-ND" xr:uid="{FB9C0F3E-259D-4D2D-8C3D-1765D4399B0E}"/>
-    <hyperlink ref="F30" tooltip="Component" display="'" xr:uid="{68770B34-DBED-40F4-BA54-4F6FFDD533EE}"/>
-    <hyperlink ref="G30" tooltip="Manufacturer" display="'" xr:uid="{53F3EAD2-E025-416C-A2BD-D633F31462EE}"/>
-    <hyperlink ref="L30" tooltip="Supplier" display="'" xr:uid="{A3DACC7C-10F4-43ED-9978-0229F5A0500B}"/>
-    <hyperlink ref="F31" r:id="rId85" tooltip="Component" display="'Linear Technology/Analog Devices" xr:uid="{593A1084-3F4E-4710-8F8A-451574CC8EAF}"/>
-    <hyperlink ref="G31" r:id="rId86" tooltip="Manufacturer" display="'LTC4414EMS8#PBF" xr:uid="{07CE0E34-B8DF-443C-AC98-0A7C7C43E880}"/>
-    <hyperlink ref="L31" r:id="rId87" tooltip="Supplier" display="'LTC4414EMS8#PBF-ND" xr:uid="{42BA36AD-97E7-4400-9DCD-4EE523614DE3}"/>
-    <hyperlink ref="F32" r:id="rId88" tooltip="Component" display="'Texas Instruments" xr:uid="{56A837F9-17B2-4512-834E-899557F011D8}"/>
-    <hyperlink ref="G32" r:id="rId89" tooltip="Manufacturer" display="'TLV70233DBVR" xr:uid="{6051A3E7-10B2-449D-BF55-4A79394BF35D}"/>
-    <hyperlink ref="L32" r:id="rId90" tooltip="Supplier" display="'296-32415-1-ND" xr:uid="{2CFD0D34-13BF-4E08-99DF-CBCE5813ACC5}"/>
-    <hyperlink ref="F33" r:id="rId91" tooltip="Component" display="'Texas Instruments" xr:uid="{335A0CF9-59AB-439A-B75E-79250C51215D}"/>
-    <hyperlink ref="G33" r:id="rId92" tooltip="Manufacturer" display="'LM2776DBVR" xr:uid="{CF6E43AD-DDA5-4527-8149-E7F1F085B698}"/>
-    <hyperlink ref="L33" r:id="rId93" tooltip="Supplier" display="'296-43957-6-ND" xr:uid="{5CDA03CF-30A3-46CC-A782-F96F6AEA6923}"/>
-    <hyperlink ref="F34" r:id="rId94" tooltip="Component" display="'Texas Instruments" xr:uid="{790BCF47-567B-433A-A3E6-208DD5633714}"/>
-    <hyperlink ref="G34" r:id="rId95" tooltip="Manufacturer" display="'LMR23625CDDAR" xr:uid="{F872609F-6665-4C50-B87E-87D341BDF3D6}"/>
-    <hyperlink ref="L34" r:id="rId96" tooltip="Supplier" display="'296-47268-1-ND" xr:uid="{90C86437-EB90-4106-80A6-B1F5E9FD07FC}"/>
-    <hyperlink ref="F35" r:id="rId97" tooltip="Component" display="'Texas Instruments" xr:uid="{B7C4B83A-24E5-4FF8-A694-88907928A62F}"/>
-    <hyperlink ref="G35" r:id="rId98" tooltip="Manufacturer" display="'OPA188AIDBVT" xr:uid="{AD129C37-10D6-4923-8270-F8205A888194}"/>
-    <hyperlink ref="L35" r:id="rId99" tooltip="Supplier" display="'296-36218-1-ND" xr:uid="{32C1E4F1-85BF-473F-A4A9-E8A451AA4FEC}"/>
-    <hyperlink ref="F36" r:id="rId100" tooltip="Component" display="'Linear Technology" xr:uid="{2F5716EF-8F58-46B1-B3D4-180340485DDD}"/>
-    <hyperlink ref="G36" r:id="rId101" tooltip="Manufacturer" display="'LT3461AES6#TRMPBF" xr:uid="{2E4D9F4C-5ACA-42F0-8186-9CFDB5679187}"/>
-    <hyperlink ref="L36" r:id="rId102" tooltip="Supplier" display="'LT3461AES6#TRMPBFCT-ND" xr:uid="{7B37BD3B-CAF8-4F06-8DAE-1C0C0F6C45AA}"/>
-    <hyperlink ref="F37" r:id="rId103" tooltip="Component" display="'TDK-Lambda Americas Inc." xr:uid="{7D85A69F-E299-47DC-BCB1-9BC81C3A92F3}"/>
-    <hyperlink ref="G37" r:id="rId104" tooltip="Manufacturer" display="'CCG152405S" xr:uid="{531F7363-CB8C-4534-8259-B47A79E614D2}"/>
-    <hyperlink ref="L37" r:id="rId105" tooltip="Supplier" display="'285-2605-ND" xr:uid="{A48B3DB0-23D7-4EFA-9F41-B12F826177EA}"/>
-    <hyperlink ref="F38" r:id="rId106" tooltip="Component" display="'TDK-Lambda Americas Inc." xr:uid="{B5EDBB88-C3E2-465F-ACEC-C191E3F478EE}"/>
-    <hyperlink ref="G38" r:id="rId107" tooltip="Manufacturer" display="'CCG302412S" xr:uid="{945C99AE-2100-4989-82D3-75781B815111}"/>
-    <hyperlink ref="L38" r:id="rId108" tooltip="Supplier" display="'285-2419-ND" xr:uid="{45CBEEB8-14F3-44EF-951D-2287D959DD87}"/>
+    <hyperlink ref="F2" r:id="rId1" tooltip="Component" display="'Taiyo Yuden" xr:uid="{0B333041-637C-4888-88C3-3881FC2072AD}"/>
+    <hyperlink ref="G2" r:id="rId2" tooltip="Manufacturer" display="'JMK316BJ106ML-T" xr:uid="{B85F84AB-A865-4C41-872B-C042E186E2F4}"/>
+    <hyperlink ref="L2" r:id="rId3" tooltip="Supplier" display="'587-5447-1-ND" xr:uid="{05F9D8CB-92B5-42FE-A71F-634C6B7D326F}"/>
+    <hyperlink ref="F3" r:id="rId4" tooltip="Component" display="'Murata Electronics North America" xr:uid="{88BE8058-204A-49D5-BA9C-ECC9EC7CD5FE}"/>
+    <hyperlink ref="G3" r:id="rId5" tooltip="Manufacturer" display="'GRM32RR71H105KA01L" xr:uid="{BA2162C7-0EA0-4BCB-807E-52B1C28BDAC4}"/>
+    <hyperlink ref="L3" r:id="rId6" tooltip="Supplier" display="'490-1863-6-ND" xr:uid="{4301D526-41B0-4B01-9540-0D4FBDA2B8A8}"/>
+    <hyperlink ref="F4" r:id="rId7" tooltip="Component" display="'TDK Corporation" xr:uid="{27553018-8573-4373-83A8-1DD1D4177B37}"/>
+    <hyperlink ref="G4" r:id="rId8" tooltip="Manufacturer" display="'C2012X6S1C106K085AC" xr:uid="{FA712CA8-B95E-4630-878F-538343DD561C}"/>
+    <hyperlink ref="L4" r:id="rId9" tooltip="Supplier" display="'445-14483-6-ND" xr:uid="{E880D0B6-12E2-48F3-9CDD-D786FCE80617}"/>
+    <hyperlink ref="F5" r:id="rId10" tooltip="Component" display="'Yageo" xr:uid="{5E5E82C4-42B9-4121-9EB9-30EF63F5F9E2}"/>
+    <hyperlink ref="G5" r:id="rId11" tooltip="Manufacturer" display="'CC0805KKX7R6BB105" xr:uid="{9ED0E619-C2AE-4170-90DA-6E319DCD81AD}"/>
+    <hyperlink ref="L5" r:id="rId12" tooltip="Supplier" display="'311-1458-6-ND" xr:uid="{5F4B0EA0-6E0D-4021-902C-DB5BA8FCBF2A}"/>
+    <hyperlink ref="F6" r:id="rId13" tooltip="Component" display="'TDK Corporation" xr:uid="{973A6823-8A54-4520-9DAC-6115EABE5D91}"/>
+    <hyperlink ref="G6" r:id="rId14" tooltip="Manufacturer" display="'C1608X5R1H684K080AB" xr:uid="{82799995-D288-4C4B-B2F9-4C1D8B064986}"/>
+    <hyperlink ref="L6" r:id="rId15" tooltip="Supplier" display="'445-7466-6-ND" xr:uid="{F964448F-4141-4239-B9DE-40970B1855D6}"/>
+    <hyperlink ref="F7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{22F52735-E174-4E7B-840C-5951A3ABC9A3}"/>
+    <hyperlink ref="G7" r:id="rId17" tooltip="Manufacturer" display="'C0805C100M4GACTU" xr:uid="{B340A79B-2567-4040-8C65-D9B65E6C926F}"/>
+    <hyperlink ref="L7" r:id="rId18" tooltip="Supplier" display="'399-9147-6-ND" xr:uid="{AE8D14F5-559A-44E2-AF1F-6E5EF8D504EC}"/>
+    <hyperlink ref="F8" r:id="rId19" tooltip="Component" display="'Murata Electronics North America" xr:uid="{39A81022-8D10-4B1A-86B6-06C7D2095F19}"/>
+    <hyperlink ref="G8" r:id="rId20" tooltip="Manufacturer" display="'GRM32ER71H475KA88L" xr:uid="{F5075297-6600-4317-BB77-129DCA8F69CA}"/>
+    <hyperlink ref="L8" r:id="rId21" tooltip="Supplier" display="'490-1864-6-ND" xr:uid="{12DC4804-3E32-435E-8B49-BDDAFAF61953}"/>
+    <hyperlink ref="F9" r:id="rId22" tooltip="Component" display="'TDK Corporation" xr:uid="{214F6013-D53D-453F-88C7-81760CE8F587}"/>
+    <hyperlink ref="G9" r:id="rId23" tooltip="Manufacturer" display="'C1608X5R1H104K080AA" xr:uid="{EB5D9A01-0DF7-42A6-BAD4-946D58014300}"/>
+    <hyperlink ref="L9" r:id="rId24" tooltip="Supplier" display="'445-7456-6-ND" xr:uid="{BFA60DA6-A114-4C10-A4D7-2BFB081EB813}"/>
+    <hyperlink ref="F10" r:id="rId25" tooltip="Component" display="'Murata Electronics North America" xr:uid="{3A9300F0-9FEC-4882-B25F-D465B6170B62}"/>
+    <hyperlink ref="G10" r:id="rId26" tooltip="Manufacturer" display="'GRM188R61A225KE34D" xr:uid="{A79C5FC8-CFFC-49D3-B532-7F4E7CFCD326}"/>
+    <hyperlink ref="L10" r:id="rId27" tooltip="Supplier" display="'490-1545-6-ND" xr:uid="{FAAA9214-F7F5-4FF6-9F0E-64AB010FE323}"/>
+    <hyperlink ref="F11" r:id="rId28" tooltip="Component" display="'KEMET" xr:uid="{3487AF6C-B11C-4F80-9C62-F124516BCBE6}"/>
+    <hyperlink ref="G11" r:id="rId29" tooltip="Manufacturer" display="'C1206C220K5GACTU" xr:uid="{F0FFD14E-371B-49D1-BFBB-2C076E937CCE}"/>
+    <hyperlink ref="L11" r:id="rId30" tooltip="Supplier" display="'399-8165-1-ND" xr:uid="{94615751-D92C-405C-8E12-68ABCB2BBBFE}"/>
+    <hyperlink ref="F12" r:id="rId31" tooltip="Component" display="'Taiyo Yuden" xr:uid="{FB15FC53-CF71-4803-BDBF-C8AE0C4306C7}"/>
+    <hyperlink ref="G12" r:id="rId32" tooltip="Manufacturer" display="'UMK325B7105KH-T" xr:uid="{A125EE28-6D77-4AC3-8B32-1DF0D71C2327}"/>
+    <hyperlink ref="L12" r:id="rId33" tooltip="Supplier" display="'587-1366-1-ND" xr:uid="{B4982206-D752-4D7C-B0BC-5A562CE8ACC1}"/>
+    <hyperlink ref="F13" r:id="rId34" tooltip="Component" display="'Taiyo Yuden" xr:uid="{C3A3F132-BDAC-4D80-B396-48C1EF6D31FD}"/>
+    <hyperlink ref="G13" r:id="rId35" tooltip="Manufacturer" display="'UMK316B7474KL-T" xr:uid="{E115805C-433A-4692-82D3-769CA63C1CA9}"/>
+    <hyperlink ref="L13" r:id="rId36" tooltip="Supplier" display="'587-1325-1-ND" xr:uid="{FCFAD5E7-8DBD-4652-A066-EE34E45B2686}"/>
+    <hyperlink ref="F14" r:id="rId37" tooltip="Component" display="'Taiyo Yuden" xr:uid="{ECB441D5-867F-440C-B9EC-E32D4B15F1C4}"/>
+    <hyperlink ref="G14" r:id="rId38" tooltip="Manufacturer" display="'EMK212B7105KG-T" xr:uid="{7C834448-5036-41C2-B5D4-3516BD1A4E58}"/>
+    <hyperlink ref="L14" r:id="rId39" tooltip="Supplier" display="'587-1283-1-ND" xr:uid="{A64722D5-4BB9-4BAA-A455-8E5AADCF6A57}"/>
+    <hyperlink ref="F15" r:id="rId40" tooltip="Component" display="'KEMET" xr:uid="{FED7FC97-5004-4E81-89BA-4A3A5D44012E}"/>
+    <hyperlink ref="G15" r:id="rId41" tooltip="Manufacturer" display="'C0805C475K4RACTU" xr:uid="{00F10A80-29B4-4F87-8C7C-5C0537CDA69D}"/>
+    <hyperlink ref="L15" r:id="rId42" tooltip="Supplier" display="'399-7415-1-ND" xr:uid="{BAE1F426-9C5F-4878-9246-27328B654CBB}"/>
+    <hyperlink ref="F16" r:id="rId43" tooltip="Component" display="'Murata Electronics North America" xr:uid="{19E1360A-2F17-4E94-B4E7-F102CE38C8AF}"/>
+    <hyperlink ref="G16" r:id="rId44" tooltip="Manufacturer" display="'GRM188R71C473KA01D" xr:uid="{C6C4EBA2-7169-4E4B-9475-24B4513152A1}"/>
+    <hyperlink ref="L16" r:id="rId45" tooltip="Supplier" display="'490-1529-6-ND" xr:uid="{6EE9FED0-0282-4EB8-B046-657C30F32AEA}"/>
+    <hyperlink ref="F17" r:id="rId46" tooltip="Component" display="'Comchip Technology" xr:uid="{16937DB7-107B-41A0-8747-D4119B2A1277}"/>
+    <hyperlink ref="G17" r:id="rId47" tooltip="Manufacturer" display="'CDBA540-HF" xr:uid="{4C74E3C8-3AC5-4C37-9065-0ECFF5B916E0}"/>
+    <hyperlink ref="L17" r:id="rId48" tooltip="Supplier" display="'641-1707-6-ND" xr:uid="{E2427DD8-B27A-4EE8-B14B-BB901FFA8378}"/>
+    <hyperlink ref="F18" r:id="rId49" tooltip="Component" display="'Pulse Electronics Power" xr:uid="{28C98674-225F-471F-AC4D-C52B0E80FE61}"/>
+    <hyperlink ref="G18" r:id="rId50" tooltip="Manufacturer" display="'PA4332.222NLT" xr:uid="{BA83074E-4BEC-4DE6-B392-79792EA8BC7C}"/>
+    <hyperlink ref="L18" r:id="rId51" tooltip="Supplier" display="'553-3290-6-ND" xr:uid="{2A847B1D-0F85-4943-8EDF-9C9F14FE64F1}"/>
+    <hyperlink ref="F19" r:id="rId52" tooltip="Component" display="'Murata Electronics North America" xr:uid="{386943B4-73BD-4DF0-B545-921E20168125}"/>
+    <hyperlink ref="G19" r:id="rId53" tooltip="Manufacturer" display="'LQH32CN470K23L" xr:uid="{309201E3-1326-48F3-9AAE-EA7942D1E223}"/>
+    <hyperlink ref="L19" r:id="rId54" tooltip="Supplier" display="'490-2497-1-ND" xr:uid="{CBD8DE3B-B3B5-4A46-8274-B15DE8E12E02}"/>
+    <hyperlink ref="F20" r:id="rId55" tooltip="Component" display="'Samtec Inc." xr:uid="{11D3532F-6BB2-4518-B1C4-D2A3A222E15A}"/>
+    <hyperlink ref="G20" r:id="rId56" tooltip="Manufacturer" display="'IPL1-104-01-L-S-RA-K" xr:uid="{A623B95B-F22F-4EEA-97B8-DFDF9E37713F}"/>
+    <hyperlink ref="L20" r:id="rId57" tooltip="Supplier" display="'SAM9597-ND" xr:uid="{1ECD7C3D-B367-4EB3-AE56-7FBA977DBEAB}"/>
+    <hyperlink ref="F21" r:id="rId58" tooltip="Component" display="'Samtec Inc." xr:uid="{D2D8E271-1E56-42C6-AFB0-FBEAC8A20144}"/>
+    <hyperlink ref="G21" r:id="rId59" tooltip="Manufacturer" display="'SSW-115-01-F-D" xr:uid="{125AE928-3845-40D6-A8E9-A2B7730BF6E1}"/>
+    <hyperlink ref="L21" r:id="rId60" tooltip="Supplier" display="'SAM10034-ND" xr:uid="{3313F678-F789-4EC6-8B7B-C0819265D223}"/>
+    <hyperlink ref="F22" r:id="rId61" tooltip="Component" display="'ON Semiconductor" xr:uid="{D3D987D1-8233-41CF-9014-72FA4E799CD0}"/>
+    <hyperlink ref="G22" r:id="rId62" tooltip="Manufacturer" display="'MCH6336-TL-E" xr:uid="{A1429247-679F-45D7-9EF9-9DA7F6DC52A4}"/>
+    <hyperlink ref="L22" r:id="rId63" tooltip="Supplier" display="'MCH6336-TL-EOSCT-ND" xr:uid="{FEF1FAED-0A21-4766-96C0-3B402C4BC637}"/>
+    <hyperlink ref="F23" r:id="rId64" tooltip="Component" display="'Panasonic Electronic Components" xr:uid="{0D162909-9DAB-4233-9305-3297248258E0}"/>
+    <hyperlink ref="G23" r:id="rId65" tooltip="Manufacturer" display="'ERJ-2RKF5603X" xr:uid="{2C6525CD-5E14-4F25-99B6-B47A407B539C}"/>
+    <hyperlink ref="L23" r:id="rId66" tooltip="Supplier" display="'P560KLCT-ND" xr:uid="{390FB0EC-39E9-4C75-998D-15A807790D46}"/>
+    <hyperlink ref="F24" r:id="rId67" tooltip="Component" display="'Vishay Dale" xr:uid="{D56B3988-00C2-4598-B96B-552D61354E19}"/>
+    <hyperlink ref="G24" r:id="rId68" tooltip="Manufacturer" display="'CRCW080588K7FKEA" xr:uid="{86563EC9-452A-405A-A73C-874D4AA71001}"/>
+    <hyperlink ref="L24" r:id="rId69" tooltip="Supplier" display="'541-88.7KCDKR-ND" xr:uid="{EFBC03F8-6215-4CB0-9D6A-7FB18FD64926}"/>
+    <hyperlink ref="F25" r:id="rId70" tooltip="Component" display="'Vishay Dale" xr:uid="{D5C79EF4-F70C-4BA9-9155-6822A516D57D}"/>
+    <hyperlink ref="G25" r:id="rId71" tooltip="Manufacturer" display="'CRCW080522K1FKEA" xr:uid="{E0863F2F-9EA2-4D2F-9ECB-D608839980DE}"/>
+    <hyperlink ref="L25" r:id="rId72" tooltip="Supplier" display="'541-22.1KCDKR-ND" xr:uid="{42808CBF-8ACB-4BE7-86C7-4CD865B508A8}"/>
+    <hyperlink ref="F26" r:id="rId73" tooltip="Component" display="'Vishay" xr:uid="{A898B7B8-A8AA-4C8A-8990-7E749E5A3C28}"/>
+    <hyperlink ref="G26" r:id="rId74" tooltip="Manufacturer" display="'CRCW0805100KFKEA" xr:uid="{2AC95F2D-9123-44B3-B76E-9E73737CD4FD}"/>
+    <hyperlink ref="L26" r:id="rId75" tooltip="Supplier" display="'CRCW0805100KFKEA/BKN" xr:uid="{F6E55921-382E-4101-9E8D-D390C2B203C1}"/>
+    <hyperlink ref="F27" r:id="rId76" tooltip="Component" display="'Vishay Dale" xr:uid="{3006368E-A0A7-457C-A686-BCF30E2870A8}"/>
+    <hyperlink ref="G27" r:id="rId77" tooltip="Manufacturer" display="'CRCW0805280KFKEA" xr:uid="{D60C2C2F-7187-4D46-8107-E49978E35C27}"/>
+    <hyperlink ref="L27" r:id="rId78" tooltip="Supplier" display="'541-280KCTR-ND" xr:uid="{AAE053EE-0D69-4FB6-8B8D-DC56D792B65C}"/>
+    <hyperlink ref="F28" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{A2A6CFF0-6B2E-4CAB-8F1F-FAE3FF3C4A87}"/>
+    <hyperlink ref="G28" r:id="rId80" tooltip="Manufacturer" display="'RC0805FR-0710KL" xr:uid="{A85DB998-E3D0-4585-9213-037C1156B633}"/>
+    <hyperlink ref="L28" r:id="rId81" tooltip="Supplier" display="'311-10.0KCRCT-ND" xr:uid="{2B38AD42-42B8-4C14-B880-88F1E5CC8E79}"/>
+    <hyperlink ref="F29" tooltip="Component" display="'" xr:uid="{7E831EBA-3563-49C2-8D6A-DE62F7D82D6E}"/>
+    <hyperlink ref="G29" tooltip="Manufacturer" display="'" xr:uid="{9D63267B-E8D1-4721-A0FA-88261C07A853}"/>
+    <hyperlink ref="L29" tooltip="Supplier" display="'" xr:uid="{574FF479-BECC-4BEA-9A70-20D2A17CCD24}"/>
+    <hyperlink ref="F30" r:id="rId82" tooltip="Component" display="'Linear Technology/Analog Devices" xr:uid="{9D202871-4EB0-45D0-A4A4-AEA7D251E3E9}"/>
+    <hyperlink ref="G30" r:id="rId83" tooltip="Manufacturer" display="'LTC4414EMS8#PBF" xr:uid="{42B59E39-3345-4E94-B77A-246D28C9B32F}"/>
+    <hyperlink ref="L30" r:id="rId84" tooltip="Supplier" display="'LTC4414EMS8#PBF-ND" xr:uid="{831D6339-D40D-4A15-A8B9-6642D683788C}"/>
+    <hyperlink ref="F31" r:id="rId85" tooltip="Component" display="'Texas Instruments" xr:uid="{8DB0AD20-7FAE-4302-8652-989FA3A73BC3}"/>
+    <hyperlink ref="G31" r:id="rId86" tooltip="Manufacturer" display="'TLV70233DBVR" xr:uid="{BBCC449F-C186-4EFE-9690-4CE0D7B954CA}"/>
+    <hyperlink ref="L31" r:id="rId87" tooltip="Supplier" display="'296-32415-1-ND" xr:uid="{51594952-5628-4D45-8806-D1FBC41FCB92}"/>
+    <hyperlink ref="F32" r:id="rId88" tooltip="Component" display="'Texas Instruments" xr:uid="{4976DAB3-A776-4813-83FC-2E24C811B2CA}"/>
+    <hyperlink ref="G32" r:id="rId89" tooltip="Manufacturer" display="'LM2776DBVR" xr:uid="{3810CEDE-8186-43D4-B18E-70D5D81CE0E3}"/>
+    <hyperlink ref="L32" r:id="rId90" tooltip="Supplier" display="'296-43957-6-ND" xr:uid="{6F07643E-10FF-446C-8FB5-63B1EBEA3916}"/>
+    <hyperlink ref="F33" r:id="rId91" tooltip="Component" display="'Texas Instruments" xr:uid="{5E19F984-41D9-4A27-8D99-C6A811E4A3C6}"/>
+    <hyperlink ref="G33" r:id="rId92" tooltip="Manufacturer" display="'LMR23625CDDAR" xr:uid="{F0985ADC-45AC-4920-BAB0-B9D068675D27}"/>
+    <hyperlink ref="L33" r:id="rId93" tooltip="Supplier" display="'296-47268-1-ND" xr:uid="{9C0F4E39-A24C-4539-9A84-5FC7F6D2F5E4}"/>
+    <hyperlink ref="F34" r:id="rId94" tooltip="Component" display="'Texas Instruments" xr:uid="{1D8B2BDD-E3D1-498C-B6E1-0E572A04CD09}"/>
+    <hyperlink ref="G34" r:id="rId95" tooltip="Manufacturer" display="'OPA188AIDBVT" xr:uid="{E40E170E-A0A3-4BEF-912C-9263C5B8F7F7}"/>
+    <hyperlink ref="L34" r:id="rId96" tooltip="Supplier" display="'296-36218-1-ND" xr:uid="{6808191F-A62C-4588-AE51-5B51A5561105}"/>
+    <hyperlink ref="F35" r:id="rId97" tooltip="Component" display="'Linear Technology" xr:uid="{2103AA88-01E3-4D0C-87F4-34E07880C317}"/>
+    <hyperlink ref="G35" r:id="rId98" tooltip="Manufacturer" display="'LT3461AES6#TRMPBF" xr:uid="{EA315F1A-209F-4D7C-9329-DC83231C981E}"/>
+    <hyperlink ref="L35" r:id="rId99" tooltip="Supplier" display="'LT3461AES6#TRMPBFCT-ND" xr:uid="{E4982975-EC2B-4031-889B-9F5B5B98723E}"/>
+    <hyperlink ref="F36" r:id="rId100" tooltip="Component" display="'TDK-Lambda Americas Inc." xr:uid="{7A0E53AC-B263-4E50-804E-D55CBCF4F8A6}"/>
+    <hyperlink ref="G36" r:id="rId101" tooltip="Manufacturer" display="'CCG152405S" xr:uid="{3D51D33D-0CEB-454D-87D8-D2AA4C130513}"/>
+    <hyperlink ref="L36" r:id="rId102" tooltip="Supplier" display="'285-2605-ND" xr:uid="{2F16F01B-8530-40A9-9554-9C88EDCE2097}"/>
+    <hyperlink ref="F37" r:id="rId103" tooltip="Component" display="'TDK-Lambda Americas Inc." xr:uid="{D1D87CAC-670F-423A-BA39-65DF92F0F578}"/>
+    <hyperlink ref="G37" r:id="rId104" tooltip="Manufacturer" display="'CCG302412S" xr:uid="{C1368B11-6719-40DB-83B6-81B9EEA161FB}"/>
+    <hyperlink ref="L37" r:id="rId105" tooltip="Supplier" display="'285-2419-ND" xr:uid="{6B09DF58-CCA7-4B6E-95B7-EBED6F5BB7E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId109"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId106"/>
 </worksheet>
 </file>
</xml_diff>